<commit_message>
Added parameters for the modifier to work nicelyDD
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ak\Documents\GitHub\44Keys\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD534CD3-97AE-47F8-B9BD-E10E0789CCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EA8F0BE-59E8-4AB4-80AA-4C9CCC5E6809}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="22845" windowHeight="18240" xr2:uid="{1A31AB80-984F-4FFD-900E-859C0DB155D7}"/>
+    <workbookView xWindow="6360" yWindow="3015" windowWidth="16950" windowHeight="13185" xr2:uid="{1A31AB80-984F-4FFD-900E-859C0DB155D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -509,7 +509,7 @@
   <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,21 +561,21 @@
         <v>4</v>
       </c>
       <c r="E2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <f>E2+F2</f>
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <f>B2*$B$18</f>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="I2">
-        <f>H2-G2</f>
+        <f t="shared" ref="I2:I14" si="0">H2-G2</f>
         <v>2</v>
       </c>
     </row>
@@ -593,21 +593,21 @@
         <v>6</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G14" si="0">E3+F3</f>
-        <v>8</v>
+        <f t="shared" ref="G3:G14" si="1">E3+F3</f>
+        <v>6</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H14" si="1">B3*$B$18</f>
-        <v>4</v>
+        <f t="shared" ref="H3:H14" si="2">B3*$B$18</f>
+        <v>2</v>
       </c>
       <c r="I3">
-        <f>H3-G3</f>
+        <f t="shared" si="0"/>
         <v>-4</v>
       </c>
     </row>
@@ -625,21 +625,21 @@
         <v>8</v>
       </c>
       <c r="E4">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="H4">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I4">
-        <f>H4-G4</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -657,21 +657,21 @@
         <v>10</v>
       </c>
       <c r="E5">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5">
-        <f t="shared" si="0"/>
-        <v>21</v>
+        <f t="shared" si="1"/>
+        <v>17</v>
       </c>
       <c r="H5">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I5">
-        <f>H5-G5</f>
+        <f t="shared" si="0"/>
         <v>-13</v>
       </c>
     </row>
@@ -680,7 +680,7 @@
         <v>11</v>
       </c>
       <c r="B6">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -689,23 +689,22 @@
         <v>13</v>
       </c>
       <c r="E6">
-        <f>100-44+132</f>
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="F6">
         <v>22</v>
       </c>
       <c r="G6">
-        <f t="shared" si="0"/>
-        <v>210</v>
+        <f t="shared" si="1"/>
+        <v>166</v>
       </c>
       <c r="H6">
-        <f t="shared" si="1"/>
-        <v>176</v>
+        <f t="shared" si="2"/>
+        <v>44</v>
       </c>
       <c r="I6">
-        <f>H6-G6</f>
-        <v>-34</v>
+        <f t="shared" si="0"/>
+        <v>-122</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -722,19 +721,18 @@
         <v>15</v>
       </c>
       <c r="E7">
-        <f>3+6</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="H7">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I7">
-        <f>H7-G7</f>
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
     </row>
@@ -752,22 +750,21 @@
         <v>17</v>
       </c>
       <c r="E8">
-        <f>4+12</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F8">
         <v>4</v>
       </c>
       <c r="G8">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="H8">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I8">
-        <f>H8-G8</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
     </row>
@@ -785,22 +782,21 @@
         <v>19</v>
       </c>
       <c r="E9">
-        <f>4+12</f>
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F9">
         <v>4</v>
       </c>
       <c r="G9">
-        <f t="shared" si="0"/>
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>16</v>
       </c>
       <c r="H9">
-        <f t="shared" si="1"/>
-        <v>8</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="I9">
-        <f>H9-G9</f>
+        <f t="shared" si="0"/>
         <v>-12</v>
       </c>
     </row>
@@ -818,21 +814,21 @@
         <v>22</v>
       </c>
       <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
       <c r="H10">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I10">
-        <f>H10-G10</f>
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
     </row>
@@ -850,21 +846,21 @@
         <v>25</v>
       </c>
       <c r="E11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="F11">
         <v>3</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
-        <v>14</v>
+        <f t="shared" si="1"/>
+        <v>12</v>
       </c>
       <c r="H11">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I11">
-        <f>H11-G11</f>
+        <f t="shared" si="0"/>
         <v>-10</v>
       </c>
     </row>
@@ -882,22 +878,21 @@
         <v>28</v>
       </c>
       <c r="E12">
-        <f>2+6</f>
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F12">
-        <v>2</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="H12">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I12">
-        <f>H12-G12</f>
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
     </row>
@@ -915,22 +910,21 @@
         <v>31</v>
       </c>
       <c r="E13">
-        <f>4+4</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="H13">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I13">
-        <f>H13-G13</f>
+        <f t="shared" si="0"/>
         <v>-5</v>
       </c>
     </row>
@@ -945,21 +939,21 @@
         <v>35</v>
       </c>
       <c r="E14">
+        <v>6</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
       <c r="H14">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="I14">
-        <f>H14-G14</f>
+        <f t="shared" si="0"/>
         <v>-6</v>
       </c>
     </row>
@@ -968,7 +962,7 @@
         <v>40</v>
       </c>
       <c r="B18">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>